<commit_message>
Add All Testcases Procedure
Add All Testcases Procedure
</commit_message>
<xml_diff>
--- a/Configuration Files/knowledges.xlsx
+++ b/Configuration Files/knowledges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Van\Datalogic_automation\HHS_project_Automation\HHS_project\bin\Debug\Configuration Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25AD0F08-D62B-4A96-83CE-B7B4D1D75FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D658C4A6-C90F-4E1B-8D86-7906EB22ADFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{13BB9B81-5739-40EC-BE52-29F9844F204D}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
-  <si>
-    <t>Testcase</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Step1</t>
   </si>
@@ -145,13 +142,25 @@
   </si>
   <si>
     <t>UPCA1AMID_UPCA1</t>
+  </si>
+  <si>
+    <t>Testcase steps</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Read UPCA</t>
+  </si>
+  <si>
+    <t>REad UPCA_AddOn2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +170,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -186,12 +203,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,168 +527,187 @@
   <dimension ref="A2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="123.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="131.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.5703125" customWidth="1"/>
+    <col min="4" max="4" width="61.5703125" customWidth="1"/>
     <col min="5" max="5" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
+      <c r="E2" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
       <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" t="s">
         <v>32</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>